<commit_message>
actualizacion estado del tp
</commit_message>
<xml_diff>
--- a/Estado TP.xlsx
+++ b/Estado TP.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>ABM Transporte</t>
   </si>
@@ -77,7 +77,10 @@
     <t>Esta hecha, falta usarla</t>
   </si>
   <si>
-    <t>Faltan numeros negativos</t>
+    <t>Probar al final</t>
+  </si>
+  <si>
+    <t>Faltan numeros negativos y patente</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,13 +422,13 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -473,13 +476,17 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -497,13 +504,13 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -518,7 +525,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
+ excepciones y actualizacion estado tp
</commit_message>
<xml_diff>
--- a/Estado TP.xlsx
+++ b/Estado TP.xlsx
@@ -80,7 +80,7 @@
     <t>Probar al final</t>
   </si>
   <si>
-    <t>Faltan numeros negativos y patente</t>
+    <t>Falta patente</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +524,7 @@
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>